<commit_message>
Add proactive auto-enrollment and debug logging to AE process
</commit_message>
<xml_diff>
--- a/projection_results_AIP_All_Eligible.xlsx
+++ b/projection_results_AIP_All_Eligible.xlsx
@@ -528,49 +528,49 @@
         <v>9426</v>
       </c>
       <c r="C2" t="n">
-        <v>9397</v>
+        <v>9405</v>
       </c>
       <c r="D2" t="n">
-        <v>8389</v>
+        <v>8333</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8927317228902841</v>
+        <v>0.8860180754917597</v>
       </c>
       <c r="F2" t="n">
-        <v>0.88998514746446</v>
+        <v>0.8840441332484616</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1000965550125164</v>
+        <v>0.1003492139685587</v>
       </c>
       <c r="H2" t="n">
-        <v>0.08908444727349883</v>
+        <v>0.08871313388499895</v>
       </c>
       <c r="I2" t="n">
-        <v>42975206.50991</v>
+        <v>42764307.097377</v>
       </c>
       <c r="J2" t="n">
-        <v>14989468.293649</v>
+        <v>14897441.3715245</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>14989468.293649</v>
+        <v>14897441.3715245</v>
       </c>
       <c r="M2" t="n">
-        <v>57964674.803559</v>
+        <v>57661748.4689015</v>
       </c>
       <c r="N2" t="n">
-        <v>798904178.3713</v>
+        <v>798735599.8913001</v>
       </c>
       <c r="O2" t="n">
-        <v>781204371.3673</v>
+        <v>781035792.8873</v>
       </c>
       <c r="P2" t="n">
-        <v>0.01876253585781407</v>
+        <v>0.01865128006508273</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.01918764006327018</v>
+        <v>0.01907395474982301</v>
       </c>
     </row>
     <row r="3">
@@ -581,49 +581,49 @@
         <v>9613</v>
       </c>
       <c r="C3" t="n">
-        <v>9591</v>
+        <v>9584</v>
       </c>
       <c r="D3" t="n">
-        <v>8568</v>
+        <v>8485</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8933375039099155</v>
+        <v>0.8853297161936561</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8912930406740872</v>
+        <v>0.882658899407053</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1040126050420168</v>
+        <v>0.1042274602239246</v>
       </c>
       <c r="H3" t="n">
-        <v>0.09270571101633206</v>
+        <v>0.09199729532924165</v>
       </c>
       <c r="I3" t="n">
-        <v>51444042.70571415</v>
+        <v>51074341.32902661</v>
       </c>
       <c r="J3" t="n">
-        <v>18655263.22220589</v>
+        <v>18511671.10224956</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>18655263.22220589</v>
+        <v>18511671.10224956</v>
       </c>
       <c r="M3" t="n">
-        <v>70099305.92792004</v>
+        <v>69586012.43127617</v>
       </c>
       <c r="N3" t="n">
-        <v>846264310.287403</v>
+        <v>845171543.037244</v>
       </c>
       <c r="O3" t="n">
-        <v>828668874.274379</v>
+        <v>827576107.02422</v>
       </c>
       <c r="P3" t="n">
-        <v>0.02204425141817726</v>
+        <v>0.02190285659136752</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.02251232524998758</v>
+        <v>0.02236854223451836</v>
       </c>
     </row>
     <row r="4">
@@ -634,49 +634,49 @@
         <v>9804</v>
       </c>
       <c r="C4" t="n">
-        <v>9777</v>
+        <v>9768</v>
       </c>
       <c r="D4" t="n">
-        <v>8754</v>
+        <v>8627</v>
       </c>
       <c r="E4" t="n">
-        <v>0.895366676894753</v>
+        <v>0.8831900081900081</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8929008567931457</v>
+        <v>0.8799469604243166</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1086189170664839</v>
+        <v>0.1088976469224528</v>
       </c>
       <c r="H4" t="n">
-        <v>0.09698592411260712</v>
+        <v>0.09582415340677275</v>
       </c>
       <c r="I4" t="n">
-        <v>60509428.09722775</v>
+        <v>59723949.76822361</v>
       </c>
       <c r="J4" t="n">
-        <v>21902260.39046314</v>
+        <v>21601006.9797773</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>21902260.39046314</v>
+        <v>21601006.9797773</v>
       </c>
       <c r="M4" t="n">
-        <v>82411688.4876909</v>
+        <v>81324956.74800092</v>
       </c>
       <c r="N4" t="n">
-        <v>892600810.3429148</v>
+        <v>889821499.5132644</v>
       </c>
       <c r="O4" t="n">
-        <v>875036894.5483382</v>
+        <v>872257583.7186878</v>
       </c>
       <c r="P4" t="n">
-        <v>0.02453757618934812</v>
+        <v>0.02427566314321819</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.02503009933286103</v>
+        <v>0.02476448171156726</v>
       </c>
     </row>
     <row r="5">
@@ -687,49 +687,49 @@
         <v>9999</v>
       </c>
       <c r="C5" t="n">
-        <v>9965</v>
+        <v>9972</v>
       </c>
       <c r="D5" t="n">
-        <v>8935</v>
+        <v>8834</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8966382338183643</v>
+        <v>0.8858804653028479</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8935893589358936</v>
+        <v>0.8834883488348835</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1124913262451035</v>
+        <v>0.1126647045506</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1005210521052105</v>
+        <v>0.09953795379537955</v>
       </c>
       <c r="I5" t="n">
-        <v>69474795.94759443</v>
+        <v>68799121.34358832</v>
       </c>
       <c r="J5" t="n">
-        <v>24620880.0356087</v>
+        <v>24398944.62936984</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>24620880.0356087</v>
+        <v>24398944.62936984</v>
       </c>
       <c r="M5" t="n">
-        <v>94095675.98320314</v>
+        <v>93198065.97295816</v>
       </c>
       <c r="N5" t="n">
-        <v>936938365.2717324</v>
+        <v>935647705.506358</v>
       </c>
       <c r="O5" t="n">
-        <v>919337142.986478</v>
+        <v>918046483.2211035</v>
       </c>
       <c r="P5" t="n">
-        <v>0.02627801459327381</v>
+        <v>0.02607706349919974</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.02678112183700907</v>
+        <v>0.02657702531985362</v>
       </c>
     </row>
     <row r="6">
@@ -740,49 +740,49 @@
         <v>10198</v>
       </c>
       <c r="C6" t="n">
-        <v>10178</v>
+        <v>10163</v>
       </c>
       <c r="D6" t="n">
-        <v>9130</v>
+        <v>9012</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8970328158773826</v>
+        <v>0.8867460395552494</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8952735830555011</v>
+        <v>0.8837026868013336</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1139167579408543</v>
+        <v>0.1144274300932091</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1019866640517749</v>
+        <v>0.1011198274171406</v>
       </c>
       <c r="I6" t="n">
-        <v>77829620.15186457</v>
+        <v>76969728.48235811</v>
       </c>
       <c r="J6" t="n">
-        <v>26033631.65407828</v>
+        <v>25719545.75328371</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>26033631.65407828</v>
+        <v>25719545.75328371</v>
       </c>
       <c r="M6" t="n">
-        <v>103863251.8059429</v>
+        <v>102689274.2356418</v>
       </c>
       <c r="N6" t="n">
-        <v>984235366.6876544</v>
+        <v>980150039.1428678</v>
       </c>
       <c r="O6" t="n">
-        <v>966527820.4875231</v>
+        <v>962442492.9427364</v>
       </c>
       <c r="P6" t="n">
-        <v>0.02645061591486177</v>
+        <v>0.02624041700368162</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.02693521190207101</v>
+        <v>0.02672320262444395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update projection results and add consolidated summary spreadsheet
</commit_message>
<xml_diff>
--- a/projection_results_AIP_All_Eligible.xlsx
+++ b/projection_results_AIP_All_Eligible.xlsx
@@ -525,52 +525,52 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>9426</v>
+        <v>9478</v>
       </c>
       <c r="C2" t="n">
-        <v>9405</v>
+        <v>9459</v>
       </c>
       <c r="D2" t="n">
-        <v>8333</v>
+        <v>8396</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8860180754917597</v>
+        <v>0.887620255840998</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8840441332484616</v>
+        <v>0.8858408947035239</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1003492139685587</v>
+        <v>0.09668375143367978</v>
       </c>
       <c r="H2" t="n">
-        <v>0.08871313388499895</v>
+        <v>0.08564642087330401</v>
       </c>
       <c r="I2" t="n">
-        <v>42764307.097377</v>
+        <v>41289012.09786491</v>
       </c>
       <c r="J2" t="n">
-        <v>14897441.3715245</v>
+        <v>14448077.45109245</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>14897441.3715245</v>
+        <v>14448077.45109245</v>
       </c>
       <c r="M2" t="n">
-        <v>57661748.4689015</v>
+        <v>55737089.54895736</v>
       </c>
       <c r="N2" t="n">
-        <v>798735599.8913001</v>
+        <v>801867174.6472001</v>
       </c>
       <c r="O2" t="n">
-        <v>781035792.8873</v>
+        <v>784167367.6432</v>
       </c>
       <c r="P2" t="n">
-        <v>0.01865128006508273</v>
+        <v>0.01801804327187881</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.01907395474982301</v>
+        <v>0.01842473692129765</v>
       </c>
     </row>
     <row r="3">
@@ -578,52 +578,52 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>9613</v>
+        <v>9666</v>
       </c>
       <c r="C3" t="n">
-        <v>9584</v>
+        <v>9648</v>
       </c>
       <c r="D3" t="n">
-        <v>8485</v>
+        <v>8564</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8853297161936561</v>
+        <v>0.8876451077943616</v>
       </c>
       <c r="F3" t="n">
-        <v>0.882658899407053</v>
+        <v>0.8859921373887855</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1042274602239246</v>
+        <v>0.1019731364521253</v>
       </c>
       <c r="H3" t="n">
-        <v>0.09199729532924165</v>
+        <v>0.09034739712145676</v>
       </c>
       <c r="I3" t="n">
-        <v>51074341.32902661</v>
+        <v>48113730.21848053</v>
       </c>
       <c r="J3" t="n">
-        <v>18511671.10224956</v>
+        <v>17590471.60814859</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>18511671.10224956</v>
+        <v>17590471.60814859</v>
       </c>
       <c r="M3" t="n">
-        <v>69586012.43127617</v>
+        <v>65704201.82662913</v>
       </c>
       <c r="N3" t="n">
-        <v>845171543.037244</v>
+        <v>838090574.9417281</v>
       </c>
       <c r="O3" t="n">
-        <v>827576107.02422</v>
+        <v>820610398.917658</v>
       </c>
       <c r="P3" t="n">
-        <v>0.02190285659136752</v>
+        <v>0.02098874767726823</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.02236854223451836</v>
+        <v>0.02143583804366786</v>
       </c>
     </row>
     <row r="4">
@@ -631,52 +631,52 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>9804</v>
+        <v>9858</v>
       </c>
       <c r="C4" t="n">
-        <v>9768</v>
+        <v>9838</v>
       </c>
       <c r="D4" t="n">
-        <v>8627</v>
+        <v>8719</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8831900081900081</v>
+        <v>0.8862573693840211</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8799469604243166</v>
+        <v>0.8844593223777643</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1088976469224528</v>
+        <v>0.1062951315653054</v>
       </c>
       <c r="H4" t="n">
-        <v>0.09582415340677275</v>
+        <v>0.09401372003630526</v>
       </c>
       <c r="I4" t="n">
-        <v>59723949.76822361</v>
+        <v>54572877.58804671</v>
       </c>
       <c r="J4" t="n">
-        <v>21601006.9797773</v>
+        <v>20500073.82904293</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>21601006.9797773</v>
+        <v>20500073.82904293</v>
       </c>
       <c r="M4" t="n">
-        <v>81324956.74800092</v>
+        <v>75072951.41708964</v>
       </c>
       <c r="N4" t="n">
-        <v>889821499.5132644</v>
+        <v>875624633.6923679</v>
       </c>
       <c r="O4" t="n">
-        <v>872257583.7186878</v>
+        <v>858175685.6864141</v>
       </c>
       <c r="P4" t="n">
-        <v>0.02427566314321819</v>
+        <v>0.02341194278945468</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.02476448171156726</v>
+        <v>0.02388796859543496</v>
       </c>
     </row>
     <row r="5">
@@ -684,52 +684,52 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>9999</v>
+        <v>10054</v>
       </c>
       <c r="C5" t="n">
-        <v>9972</v>
+        <v>10027</v>
       </c>
       <c r="D5" t="n">
-        <v>8834</v>
+        <v>8900</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8858804653028479</v>
+        <v>0.8876034706293009</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8834883488348835</v>
+        <v>0.8852198130097474</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1126647045506</v>
+        <v>0.1095103629387546</v>
       </c>
       <c r="H5" t="n">
-        <v>0.09953795379537955</v>
+        <v>0.0969407430032739</v>
       </c>
       <c r="I5" t="n">
-        <v>68799121.34358832</v>
+        <v>60694383.83057234</v>
       </c>
       <c r="J5" t="n">
-        <v>24398944.62936984</v>
+        <v>23227702.42889509</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>24398944.62936984</v>
+        <v>23227702.42889509</v>
       </c>
       <c r="M5" t="n">
-        <v>93198065.97295816</v>
+        <v>83922086.25946742</v>
       </c>
       <c r="N5" t="n">
-        <v>935647705.506358</v>
+        <v>914123490.6623945</v>
       </c>
       <c r="O5" t="n">
-        <v>918046483.2211035</v>
+        <v>896637385.1994213</v>
       </c>
       <c r="P5" t="n">
-        <v>0.02607706349919974</v>
+        <v>0.0254098080469016</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.02657702531985362</v>
+        <v>0.02590534681277986</v>
       </c>
     </row>
     <row r="6">
@@ -737,52 +737,52 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>10198</v>
+        <v>10254</v>
       </c>
       <c r="C6" t="n">
-        <v>10163</v>
+        <v>10233</v>
       </c>
       <c r="D6" t="n">
-        <v>9012</v>
+        <v>9083</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8867460395552494</v>
+        <v>0.8876184892016027</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8837026868013336</v>
+        <v>0.8858006631558416</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1144274300932091</v>
+        <v>0.1088021642591696</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1011198274171406</v>
+        <v>0.09637702925356322</v>
       </c>
       <c r="I6" t="n">
-        <v>76969728.48235811</v>
+        <v>63966942.7227219</v>
       </c>
       <c r="J6" t="n">
-        <v>25719545.75328371</v>
+        <v>24492884.87752456</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>25719545.75328371</v>
+        <v>24492884.87752456</v>
       </c>
       <c r="M6" t="n">
-        <v>102689274.2356418</v>
+        <v>88459827.60024647</v>
       </c>
       <c r="N6" t="n">
-        <v>980150039.1428678</v>
+        <v>957320807.0430477</v>
       </c>
       <c r="O6" t="n">
-        <v>962442492.9427364</v>
+        <v>939728981.1698662</v>
       </c>
       <c r="P6" t="n">
-        <v>0.02624041700368162</v>
+        <v>0.02558482454087431</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.02672320262444395</v>
+        <v>0.02606377516103998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix AI enrollment flag preservation for existing participants in plan_rules.py
</commit_message>
<xml_diff>
--- a/projection_results_AIP_All_Eligible.xlsx
+++ b/projection_results_AIP_All_Eligible.xlsx
@@ -528,49 +528,49 @@
         <v>9478</v>
       </c>
       <c r="C2" t="n">
-        <v>9459</v>
+        <v>9455</v>
       </c>
       <c r="D2" t="n">
-        <v>8396</v>
+        <v>8375</v>
       </c>
       <c r="E2" t="n">
-        <v>0.887620255840998</v>
+        <v>0.8857747223691169</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8858408947035239</v>
+        <v>0.8836252373918548</v>
       </c>
       <c r="G2" t="n">
-        <v>0.09668375143367978</v>
+        <v>0.09689384242872673</v>
       </c>
       <c r="H2" t="n">
-        <v>0.08564642087330401</v>
+        <v>0.08561784451789264</v>
       </c>
       <c r="I2" t="n">
-        <v>41289012.09786491</v>
+        <v>41234906.25223832</v>
       </c>
       <c r="J2" t="n">
-        <v>14448077.45109245</v>
+        <v>14421586.78406116</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>14448077.45109245</v>
+        <v>14421586.78406116</v>
       </c>
       <c r="M2" t="n">
-        <v>55737089.54895736</v>
+        <v>55656493.03629947</v>
       </c>
       <c r="N2" t="n">
-        <v>801867174.6472001</v>
+        <v>800568137.6472001</v>
       </c>
       <c r="O2" t="n">
-        <v>784167367.6432</v>
+        <v>782868330.6432</v>
       </c>
       <c r="P2" t="n">
-        <v>0.01801804327187881</v>
+        <v>0.018014190305456</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.01842473692129765</v>
+        <v>0.01842147168248901</v>
       </c>
     </row>
     <row r="3">
@@ -581,49 +581,49 @@
         <v>9666</v>
       </c>
       <c r="C3" t="n">
-        <v>9648</v>
+        <v>9647</v>
       </c>
       <c r="D3" t="n">
-        <v>8564</v>
+        <v>8557</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8876451077943616</v>
+        <v>0.8870115061677205</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8859921373887855</v>
+        <v>0.8852679495137595</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1019731364521253</v>
+        <v>0.1020477647857244</v>
       </c>
       <c r="H3" t="n">
-        <v>0.09034739712145676</v>
+        <v>0.09033961548432071</v>
       </c>
       <c r="I3" t="n">
-        <v>48113730.21848053</v>
+        <v>48109582.45102569</v>
       </c>
       <c r="J3" t="n">
-        <v>17590471.60814859</v>
+        <v>17588976.84787663</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>17590471.60814859</v>
+        <v>17588976.84787663</v>
       </c>
       <c r="M3" t="n">
-        <v>65704201.82662913</v>
+        <v>65698559.29890232</v>
       </c>
       <c r="N3" t="n">
-        <v>838090574.9417281</v>
+        <v>838121313.564728</v>
       </c>
       <c r="O3" t="n">
-        <v>820610398.917658</v>
+        <v>820641137.540658</v>
       </c>
       <c r="P3" t="n">
-        <v>0.02098874767726823</v>
+        <v>0.02098619443653873</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.02143583804366786</v>
+        <v>0.0214332136707017</v>
       </c>
     </row>
     <row r="4">
@@ -634,49 +634,49 @@
         <v>9858</v>
       </c>
       <c r="C4" t="n">
-        <v>9838</v>
+        <v>9840</v>
       </c>
       <c r="D4" t="n">
-        <v>8719</v>
+        <v>8723</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8862573693840211</v>
+        <v>0.8864837398373984</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8844593223777643</v>
+        <v>0.8848650841955772</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1062951315653054</v>
+        <v>0.1062957128902854</v>
       </c>
       <c r="H4" t="n">
-        <v>0.09401372003630526</v>
+        <v>0.09405736493629131</v>
       </c>
       <c r="I4" t="n">
-        <v>54572877.58804671</v>
+        <v>54616763.50503325</v>
       </c>
       <c r="J4" t="n">
-        <v>20500073.82904293</v>
+        <v>20522613.28469532</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>20500073.82904293</v>
+        <v>20522613.28469532</v>
       </c>
       <c r="M4" t="n">
-        <v>75072951.41708964</v>
+        <v>75139376.78972858</v>
       </c>
       <c r="N4" t="n">
-        <v>875624633.6923679</v>
+        <v>876530452.3962009</v>
       </c>
       <c r="O4" t="n">
-        <v>858175685.6864141</v>
+        <v>859081504.3902471</v>
       </c>
       <c r="P4" t="n">
-        <v>0.02341194278945468</v>
+        <v>0.02341346296479713</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.02388796859543496</v>
+        <v>0.02388901772394893</v>
       </c>
     </row>
     <row r="5">
@@ -687,49 +687,49 @@
         <v>10054</v>
       </c>
       <c r="C5" t="n">
-        <v>10027</v>
+        <v>10032</v>
       </c>
       <c r="D5" t="n">
-        <v>8900</v>
+        <v>8909</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8876034706293009</v>
+        <v>0.8880582137161085</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8852198130097474</v>
+        <v>0.8861149791127909</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1095103629387546</v>
+        <v>0.1093961613107875</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0969407430032739</v>
+        <v>0.09693757719492795</v>
       </c>
       <c r="I5" t="n">
-        <v>60694383.83057234</v>
+        <v>60672123.38640694</v>
       </c>
       <c r="J5" t="n">
-        <v>23227702.42889509</v>
+        <v>23217186.5988863</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>23227702.42889509</v>
+        <v>23217186.5988863</v>
       </c>
       <c r="M5" t="n">
-        <v>83922086.25946742</v>
+        <v>83889309.98529324</v>
       </c>
       <c r="N5" t="n">
-        <v>914123490.6623945</v>
+        <v>914302919.6242424</v>
       </c>
       <c r="O5" t="n">
-        <v>896637385.1994213</v>
+        <v>896816814.1612692</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0254098080469016</v>
+        <v>0.02539331998242774</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.02590534681277986</v>
+        <v>0.02588843812055389</v>
       </c>
     </row>
     <row r="6">
@@ -740,49 +740,49 @@
         <v>10254</v>
       </c>
       <c r="C6" t="n">
-        <v>10233</v>
+        <v>10235</v>
       </c>
       <c r="D6" t="n">
-        <v>9083</v>
+        <v>9057</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8876184892016027</v>
+        <v>0.884904738641915</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8858006631558416</v>
+        <v>0.8832650672908133</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1088021642591696</v>
+        <v>0.1090150774465601</v>
       </c>
       <c r="H6" t="n">
-        <v>0.09637702925356322</v>
+        <v>0.0962892097165491</v>
       </c>
       <c r="I6" t="n">
-        <v>63966942.7227219</v>
+        <v>63804904.40937157</v>
       </c>
       <c r="J6" t="n">
-        <v>24492884.87752456</v>
+        <v>24412498.54468551</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>24492884.87752456</v>
+        <v>24412498.54468551</v>
       </c>
       <c r="M6" t="n">
-        <v>88459827.60024647</v>
+        <v>88217402.95405708</v>
       </c>
       <c r="N6" t="n">
-        <v>957320807.0430477</v>
+        <v>955199529.3546511</v>
       </c>
       <c r="O6" t="n">
-        <v>939728981.1698662</v>
+        <v>937607703.4814696</v>
       </c>
       <c r="P6" t="n">
-        <v>0.02558482454087431</v>
+        <v>0.02555748594346461</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.02606377516103998</v>
+        <v>0.02603700721958497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor plan rules into modular components and add response logic
</commit_message>
<xml_diff>
--- a/projection_results_AIP_All_Eligible.xlsx
+++ b/projection_results_AIP_All_Eligible.xlsx
@@ -528,49 +528,49 @@
         <v>9478</v>
       </c>
       <c r="C2" t="n">
-        <v>9455</v>
+        <v>9458</v>
       </c>
       <c r="D2" t="n">
-        <v>8375</v>
+        <v>7574</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8857747223691169</v>
+        <v>0.8008035525481074</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8836252373918548</v>
+        <v>0.7991137370753324</v>
       </c>
       <c r="G2" t="n">
-        <v>0.09689384242872673</v>
+        <v>0.1028346976498548</v>
       </c>
       <c r="H2" t="n">
-        <v>0.08561784451789264</v>
+        <v>0.08217661953998734</v>
       </c>
       <c r="I2" t="n">
-        <v>41234906.25223832</v>
+        <v>39239770.164845</v>
       </c>
       <c r="J2" t="n">
-        <v>14421586.78406116</v>
+        <v>13420220.8417585</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>14421586.78406116</v>
+        <v>13420220.8417585</v>
       </c>
       <c r="M2" t="n">
-        <v>55656493.03629947</v>
+        <v>52659991.0066035</v>
       </c>
       <c r="N2" t="n">
-        <v>800568137.6472001</v>
+        <v>800122294.0972</v>
       </c>
       <c r="O2" t="n">
-        <v>782868330.6432</v>
+        <v>782422487.0932001</v>
       </c>
       <c r="P2" t="n">
-        <v>0.018014190305456</v>
+        <v>0.0167727120476013</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.01842147168248901</v>
+        <v>0.01715214102756216</v>
       </c>
     </row>
     <row r="3">
@@ -581,49 +581,49 @@
         <v>9666</v>
       </c>
       <c r="C3" t="n">
-        <v>9647</v>
+        <v>9637</v>
       </c>
       <c r="D3" t="n">
-        <v>8557</v>
+        <v>7551</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8870115061677205</v>
+        <v>0.7835425962436443</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8852679495137595</v>
+        <v>0.7811918063314711</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1020477647857244</v>
+        <v>0.1028830618461131</v>
       </c>
       <c r="H3" t="n">
-        <v>0.09033961548432071</v>
+        <v>0.08037140492447756</v>
       </c>
       <c r="I3" t="n">
-        <v>48109582.45102569</v>
+        <v>40538728.96122567</v>
       </c>
       <c r="J3" t="n">
-        <v>17588976.84787663</v>
+        <v>13799638.26741243</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>17588976.84787663</v>
+        <v>13799638.26741243</v>
       </c>
       <c r="M3" t="n">
-        <v>65698559.29890232</v>
+        <v>54338367.2286381</v>
       </c>
       <c r="N3" t="n">
-        <v>838121313.564728</v>
+        <v>835784763.7231281</v>
       </c>
       <c r="O3" t="n">
-        <v>820641137.540658</v>
+        <v>818304587.6990581</v>
       </c>
       <c r="P3" t="n">
-        <v>0.02098619443653873</v>
+        <v>0.01651099525425647</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.0214332136707017</v>
+        <v>0.01686369412423168</v>
       </c>
     </row>
     <row r="4">
@@ -637,46 +637,46 @@
         <v>9840</v>
       </c>
       <c r="D4" t="n">
-        <v>8723</v>
+        <v>7543</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8864837398373984</v>
+        <v>0.7665650406504065</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8848650841955772</v>
+        <v>0.7651653479407587</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1062957128902854</v>
+        <v>0.1029497547394936</v>
       </c>
       <c r="H4" t="n">
-        <v>0.09405736493629131</v>
+        <v>0.07877358490566039</v>
       </c>
       <c r="I4" t="n">
-        <v>54616763.50503325</v>
+        <v>42014448.3095379</v>
       </c>
       <c r="J4" t="n">
-        <v>20522613.28469532</v>
+        <v>14217426.49631654</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>20522613.28469532</v>
+        <v>14217426.49631654</v>
       </c>
       <c r="M4" t="n">
-        <v>75139376.78972858</v>
+        <v>56231874.80585443</v>
       </c>
       <c r="N4" t="n">
-        <v>876530452.3962009</v>
+        <v>874054288.5903099</v>
       </c>
       <c r="O4" t="n">
-        <v>859081504.3902471</v>
+        <v>856605340.5843561</v>
       </c>
       <c r="P4" t="n">
-        <v>0.02341346296479713</v>
+        <v>0.01626606800276291</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.02388901772394893</v>
+        <v>0.01659740585625785</v>
       </c>
     </row>
     <row r="5">
@@ -687,49 +687,49 @@
         <v>10054</v>
       </c>
       <c r="C5" t="n">
-        <v>10032</v>
+        <v>10034</v>
       </c>
       <c r="D5" t="n">
-        <v>8909</v>
+        <v>7534</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8880582137161085</v>
+        <v>0.7508471197927048</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8861149791127909</v>
+        <v>0.7493534911478019</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1093961613107875</v>
+        <v>0.1030222989116007</v>
       </c>
       <c r="H5" t="n">
-        <v>0.09693757719492795</v>
+        <v>0.07720011935548041</v>
       </c>
       <c r="I5" t="n">
-        <v>60672123.38640694</v>
+        <v>43535019.83059579</v>
       </c>
       <c r="J5" t="n">
-        <v>23217186.5988863</v>
+        <v>14644484.75463068</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>23217186.5988863</v>
+        <v>14644484.75463068</v>
       </c>
       <c r="M5" t="n">
-        <v>83889309.98529324</v>
+        <v>58179504.58522647</v>
       </c>
       <c r="N5" t="n">
-        <v>914302919.6242424</v>
+        <v>913242019.3379748</v>
       </c>
       <c r="O5" t="n">
-        <v>896816814.1612692</v>
+        <v>895755913.8750015</v>
       </c>
       <c r="P5" t="n">
-        <v>0.02539331998242774</v>
+        <v>0.01603571062712021</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.02588843812055389</v>
+        <v>0.01634874470577512</v>
       </c>
     </row>
     <row r="6">
@@ -740,49 +740,49 @@
         <v>10254</v>
       </c>
       <c r="C6" t="n">
-        <v>10235</v>
+        <v>10228</v>
       </c>
       <c r="D6" t="n">
-        <v>9057</v>
+        <v>7523</v>
       </c>
       <c r="E6" t="n">
-        <v>0.884904738641915</v>
+        <v>0.7355299178725069</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8832650672908133</v>
+        <v>0.7336649112541447</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1090150774465601</v>
+        <v>0.1030931809118703</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0962892097165491</v>
+        <v>0.07563584942461479</v>
       </c>
       <c r="I6" t="n">
-        <v>63804904.40937157</v>
+        <v>45146428.42506469</v>
       </c>
       <c r="J6" t="n">
-        <v>24412498.54468551</v>
+        <v>15078985.98419153</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>24412498.54468551</v>
+        <v>15078985.98419153</v>
       </c>
       <c r="M6" t="n">
-        <v>88217402.95405708</v>
+        <v>60225414.4092562</v>
       </c>
       <c r="N6" t="n">
-        <v>955199529.3546511</v>
+        <v>954929691.5795953</v>
       </c>
       <c r="O6" t="n">
-        <v>937607703.4814696</v>
+        <v>937337865.7064139</v>
       </c>
       <c r="P6" t="n">
-        <v>0.02555748594346461</v>
+        <v>0.01579067665101987</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.02603700721958497</v>
+        <v>0.01608703386033319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix auto-increase enrollment flags and add debug logging for participation tracking
</commit_message>
<xml_diff>
--- a/projection_results_AIP_All_Eligible.xlsx
+++ b/projection_results_AIP_All_Eligible.xlsx
@@ -528,49 +528,49 @@
         <v>9478</v>
       </c>
       <c r="C2" t="n">
-        <v>9458</v>
+        <v>9463</v>
       </c>
       <c r="D2" t="n">
-        <v>7574</v>
+        <v>8393</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8008035525481074</v>
+        <v>0.8869280355067104</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7991137370753324</v>
+        <v>0.8855243722304283</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1028346976498548</v>
+        <v>0.09671184592974379</v>
       </c>
       <c r="H2" t="n">
-        <v>0.08217661953998734</v>
+        <v>0.08564069665418225</v>
       </c>
       <c r="I2" t="n">
-        <v>39239770.164845</v>
+        <v>41239758.28268903</v>
       </c>
       <c r="J2" t="n">
-        <v>13420220.8417585</v>
+        <v>14425047.08800052</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>13420220.8417585</v>
+        <v>14425047.08800052</v>
       </c>
       <c r="M2" t="n">
-        <v>52659991.0066035</v>
+        <v>55664805.37068957</v>
       </c>
       <c r="N2" t="n">
-        <v>800122294.0972</v>
+        <v>800750889.2872001</v>
       </c>
       <c r="O2" t="n">
-        <v>782422487.0932001</v>
+        <v>783051082.2832</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0167727120476013</v>
+        <v>0.01801440033471731</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.01715214102756216</v>
+        <v>0.0184215914061958</v>
       </c>
     </row>
     <row r="3">
@@ -581,49 +581,49 @@
         <v>9666</v>
       </c>
       <c r="C3" t="n">
-        <v>9637</v>
+        <v>9652</v>
       </c>
       <c r="D3" t="n">
-        <v>7551</v>
+        <v>8568</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7835425962436443</v>
+        <v>0.8876916701201824</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7811918063314711</v>
+        <v>0.8864059590316573</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1028830618461131</v>
+        <v>0.1019541322918984</v>
       </c>
       <c r="H3" t="n">
-        <v>0.08037140492447756</v>
+        <v>0.09037275041144063</v>
       </c>
       <c r="I3" t="n">
-        <v>40538728.96122567</v>
+        <v>48077747.45953142</v>
       </c>
       <c r="J3" t="n">
-        <v>13799638.26741243</v>
+        <v>17574124.66950491</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>13799638.26741243</v>
+        <v>17574124.66950491</v>
       </c>
       <c r="M3" t="n">
-        <v>54338367.2286381</v>
+        <v>65651872.12903633</v>
       </c>
       <c r="N3" t="n">
-        <v>835784763.7231281</v>
+        <v>836946297.5090281</v>
       </c>
       <c r="O3" t="n">
-        <v>818304587.6990581</v>
+        <v>819466121.4849579</v>
       </c>
       <c r="P3" t="n">
-        <v>0.01651099525425647</v>
+        <v>0.02099791195899919</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.01686369412423168</v>
+        <v>0.02144582211362047</v>
       </c>
     </row>
     <row r="4">
@@ -634,49 +634,49 @@
         <v>9858</v>
       </c>
       <c r="C4" t="n">
-        <v>9840</v>
+        <v>9836</v>
       </c>
       <c r="D4" t="n">
-        <v>7543</v>
+        <v>8719</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7665650406504065</v>
+        <v>0.8864375762505083</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7651653479407587</v>
+        <v>0.8844593223777643</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1029497547394936</v>
+        <v>0.1063217547815781</v>
       </c>
       <c r="H4" t="n">
-        <v>0.07877358490566039</v>
+        <v>0.09403726718812941</v>
       </c>
       <c r="I4" t="n">
-        <v>42014448.3095379</v>
+        <v>54561128.47940587</v>
       </c>
       <c r="J4" t="n">
-        <v>14217426.49631654</v>
+        <v>20495893.04877832</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>14217426.49631654</v>
+        <v>20495893.04877832</v>
       </c>
       <c r="M4" t="n">
-        <v>56231874.80585443</v>
+        <v>75057021.52818419</v>
       </c>
       <c r="N4" t="n">
-        <v>874054288.5903099</v>
+        <v>875020684.362587</v>
       </c>
       <c r="O4" t="n">
-        <v>856605340.5843561</v>
+        <v>857571736.3566331</v>
       </c>
       <c r="P4" t="n">
-        <v>0.01626606800276291</v>
+        <v>0.02342332405971483</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.01659740585625785</v>
+        <v>0.02389991668318558</v>
       </c>
     </row>
     <row r="5">
@@ -687,49 +687,49 @@
         <v>10054</v>
       </c>
       <c r="C5" t="n">
-        <v>10034</v>
+        <v>10032</v>
       </c>
       <c r="D5" t="n">
-        <v>7534</v>
+        <v>8902</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7508471197927048</v>
+        <v>0.8873604465709729</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7493534911478019</v>
+        <v>0.8854187388104238</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1030222989116007</v>
+        <v>0.1094883113450708</v>
       </c>
       <c r="H5" t="n">
-        <v>0.07720011935548041</v>
+        <v>0.09694300254563555</v>
       </c>
       <c r="I5" t="n">
-        <v>43535019.83059579</v>
+        <v>60667658.19851614</v>
       </c>
       <c r="J5" t="n">
-        <v>14644484.75463068</v>
+        <v>23216084.20014448</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>14644484.75463068</v>
+        <v>23216084.20014448</v>
       </c>
       <c r="M5" t="n">
-        <v>58179504.58522647</v>
+        <v>83883742.3986606</v>
       </c>
       <c r="N5" t="n">
-        <v>913242019.3379748</v>
+        <v>914085108.69052</v>
       </c>
       <c r="O5" t="n">
-        <v>895755913.8750015</v>
+        <v>896599003.2275469</v>
       </c>
       <c r="P5" t="n">
-        <v>0.01603571062712021</v>
+        <v>0.02539816476542634</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.01634874470577512</v>
+        <v>0.02589349766904937</v>
       </c>
     </row>
     <row r="6">
@@ -740,49 +740,49 @@
         <v>10254</v>
       </c>
       <c r="C6" t="n">
-        <v>10228</v>
+        <v>10236</v>
       </c>
       <c r="D6" t="n">
-        <v>7523</v>
+        <v>9104</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7355299178725069</v>
+        <v>0.889409925752247</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7336649112541447</v>
+        <v>0.8878486444314414</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1030931809118703</v>
+        <v>0.1086977081952903</v>
       </c>
       <c r="H6" t="n">
-        <v>0.07563584942461479</v>
+        <v>0.09650711287399286</v>
       </c>
       <c r="I6" t="n">
-        <v>45146428.42506469</v>
+        <v>64007671.86784674</v>
       </c>
       <c r="J6" t="n">
-        <v>15078985.98419153</v>
+        <v>24515046.37498279</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>15078985.98419153</v>
+        <v>24515046.37498279</v>
       </c>
       <c r="M6" t="n">
-        <v>60225414.4092562</v>
+        <v>88522718.24282953</v>
       </c>
       <c r="N6" t="n">
-        <v>954929691.5795953</v>
+        <v>955327879.892617</v>
       </c>
       <c r="O6" t="n">
-        <v>937337865.7064139</v>
+        <v>937736054.0194355</v>
       </c>
       <c r="P6" t="n">
-        <v>0.01579067665101987</v>
+        <v>0.02566139530831905</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.01608703386033319</v>
+        <v>0.02614280027935738</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Excel files to gitignore and remove existing xlsx files from tracking
</commit_message>
<xml_diff>
--- a/projection_results_AIP_All_Eligible.xlsx
+++ b/projection_results_AIP_All_Eligible.xlsx
@@ -528,49 +528,49 @@
         <v>9478</v>
       </c>
       <c r="C2" t="n">
-        <v>9463</v>
+        <v>9465</v>
       </c>
       <c r="D2" t="n">
-        <v>8393</v>
+        <v>8384</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8869280355067104</v>
+        <v>0.8857897517168516</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8855243722304283</v>
+        <v>0.8845748048111416</v>
       </c>
       <c r="G2" t="n">
-        <v>0.09671184592974379</v>
+        <v>0.09679007923257567</v>
       </c>
       <c r="H2" t="n">
-        <v>0.08564069665418225</v>
+        <v>0.08561806544481057</v>
       </c>
       <c r="I2" t="n">
-        <v>41239758.28268903</v>
+        <v>41250664.96178105</v>
       </c>
       <c r="J2" t="n">
-        <v>14425047.08800052</v>
+        <v>14430500.42754652</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>14425047.08800052</v>
+        <v>14430500.42754652</v>
       </c>
       <c r="M2" t="n">
-        <v>55664805.37068957</v>
+        <v>55681165.38932757</v>
       </c>
       <c r="N2" t="n">
-        <v>800750889.2872001</v>
+        <v>801737041.7372</v>
       </c>
       <c r="O2" t="n">
-        <v>783051082.2832</v>
+        <v>784037234.7332001</v>
       </c>
       <c r="P2" t="n">
-        <v>0.01801440033471731</v>
+        <v>0.0179990441707403</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.0184215914061958</v>
+        <v>0.018405376413605</v>
       </c>
     </row>
     <row r="3">
@@ -581,49 +581,49 @@
         <v>9666</v>
       </c>
       <c r="C3" t="n">
-        <v>9652</v>
+        <v>9648</v>
       </c>
       <c r="D3" t="n">
-        <v>8568</v>
+        <v>8554</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8876916701201824</v>
+        <v>0.886608623548922</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8864059590316573</v>
+        <v>0.8849575832816057</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1019541322918984</v>
+        <v>0.101949910499804</v>
       </c>
       <c r="H3" t="n">
-        <v>0.09037275041144063</v>
+        <v>0.09022134641168254</v>
       </c>
       <c r="I3" t="n">
-        <v>48077747.45953142</v>
+        <v>48011620.77939813</v>
       </c>
       <c r="J3" t="n">
-        <v>17574124.66950491</v>
+        <v>17541061.32943826</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>17574124.66950491</v>
+        <v>17541061.32943826</v>
       </c>
       <c r="M3" t="n">
-        <v>65651872.12903633</v>
+        <v>65552682.10883638</v>
       </c>
       <c r="N3" t="n">
-        <v>836946297.5090281</v>
+        <v>837547624.534428</v>
       </c>
       <c r="O3" t="n">
-        <v>819466121.4849579</v>
+        <v>820067448.510358</v>
       </c>
       <c r="P3" t="n">
-        <v>0.02099791195899919</v>
+        <v>0.02094335989453603</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.02144582211362047</v>
+        <v>0.02138977880575723</v>
       </c>
     </row>
     <row r="4">
@@ -634,49 +634,49 @@
         <v>9858</v>
       </c>
       <c r="C4" t="n">
-        <v>9836</v>
+        <v>9842</v>
       </c>
       <c r="D4" t="n">
-        <v>8719</v>
+        <v>8741</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8864375762505083</v>
+        <v>0.8881324933956513</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8844593223777643</v>
+        <v>0.8866910123757354</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1063217547815781</v>
+        <v>0.1061872908635677</v>
       </c>
       <c r="H4" t="n">
-        <v>0.09403726718812941</v>
+        <v>0.09415531643725347</v>
       </c>
       <c r="I4" t="n">
-        <v>54561128.47940587</v>
+        <v>54607314.52462393</v>
       </c>
       <c r="J4" t="n">
-        <v>20495893.04877832</v>
+        <v>20518986.07138735</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>20495893.04877832</v>
+        <v>20518986.07138735</v>
       </c>
       <c r="M4" t="n">
-        <v>75057021.52818419</v>
+        <v>75126300.5960113</v>
       </c>
       <c r="N4" t="n">
-        <v>875020684.362587</v>
+        <v>875630888.769419</v>
       </c>
       <c r="O4" t="n">
-        <v>857571736.3566331</v>
+        <v>858181940.7634652</v>
       </c>
       <c r="P4" t="n">
-        <v>0.02342332405971483</v>
+        <v>0.02343337396448407</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.02389991668318558</v>
+        <v>0.02390983204928902</v>
       </c>
     </row>
     <row r="5">
@@ -687,49 +687,49 @@
         <v>10054</v>
       </c>
       <c r="C5" t="n">
-        <v>10032</v>
+        <v>10033</v>
       </c>
       <c r="D5" t="n">
-        <v>8902</v>
+        <v>8884</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8873604465709729</v>
+        <v>0.8854779228545799</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8854187388104238</v>
+        <v>0.8836284066043366</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1094883113450708</v>
+        <v>0.1096290891937461</v>
       </c>
       <c r="H5" t="n">
-        <v>0.09694300254563555</v>
+        <v>0.09687137740175458</v>
       </c>
       <c r="I5" t="n">
-        <v>60667658.19851614</v>
+        <v>60627454.10565276</v>
       </c>
       <c r="J5" t="n">
-        <v>23216084.20014448</v>
+        <v>23195982.15371279</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>23216084.20014448</v>
+        <v>23195982.15371279</v>
       </c>
       <c r="M5" t="n">
-        <v>83883742.3986606</v>
+        <v>83823436.25936554</v>
       </c>
       <c r="N5" t="n">
-        <v>914085108.69052</v>
+        <v>914110715.330657</v>
       </c>
       <c r="O5" t="n">
-        <v>896599003.2275469</v>
+        <v>896624609.8676838</v>
       </c>
       <c r="P5" t="n">
-        <v>0.02539816476542634</v>
+        <v>0.02537546247373571</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.02589349766904937</v>
+        <v>0.02587033848773776</v>
       </c>
     </row>
     <row r="6">
@@ -740,49 +740,49 @@
         <v>10254</v>
       </c>
       <c r="C6" t="n">
-        <v>10236</v>
+        <v>10231</v>
       </c>
       <c r="D6" t="n">
-        <v>9104</v>
+        <v>9096</v>
       </c>
       <c r="E6" t="n">
-        <v>0.889409925752247</v>
+        <v>0.889062652722119</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8878486444314414</v>
+        <v>0.8870684610883558</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1086977081952903</v>
+        <v>0.1086865141011976</v>
       </c>
       <c r="H6" t="n">
-        <v>0.09650711287399286</v>
+        <v>0.09641237880480726</v>
       </c>
       <c r="I6" t="n">
-        <v>64007671.86784674</v>
+        <v>63928479.04605511</v>
       </c>
       <c r="J6" t="n">
-        <v>24515046.37498279</v>
+        <v>24475449.96408697</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>24515046.37498279</v>
+        <v>24475449.96408697</v>
       </c>
       <c r="M6" t="n">
-        <v>88522718.24282953</v>
+        <v>88403929.01014209</v>
       </c>
       <c r="N6" t="n">
-        <v>955327879.892617</v>
+        <v>955558181.6979581</v>
       </c>
       <c r="O6" t="n">
-        <v>937736054.0194355</v>
+        <v>937966355.8247766</v>
       </c>
       <c r="P6" t="n">
-        <v>0.02566139530831905</v>
+        <v>0.0256137725916342</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.02614280027935738</v>
+        <v>0.02609416618420722</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add age calculation and fix tenure for new hires in projection utils
</commit_message>
<xml_diff>
--- a/projection_results_AIP_All_Eligible.xlsx
+++ b/projection_results_AIP_All_Eligible.xlsx
@@ -525,52 +525,52 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>9478</v>
+        <v>102</v>
       </c>
       <c r="C2" t="n">
-        <v>9465</v>
+        <v>102</v>
       </c>
       <c r="D2" t="n">
-        <v>8384</v>
+        <v>86</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8857897517168516</v>
+        <v>0.8431372549019608</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8845748048111416</v>
+        <v>0.8431372549019608</v>
       </c>
       <c r="G2" t="n">
-        <v>0.09679007923257567</v>
+        <v>0.09930466255509107</v>
       </c>
       <c r="H2" t="n">
-        <v>0.08561806544481057</v>
+        <v>0.08372746058566501</v>
       </c>
       <c r="I2" t="n">
-        <v>41250664.96178105</v>
+        <v>458202.2395800996</v>
       </c>
       <c r="J2" t="n">
-        <v>14430500.42754652</v>
+        <v>166487.1199910498</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>14430500.42754652</v>
+        <v>166487.1199910498</v>
       </c>
       <c r="M2" t="n">
-        <v>55681165.38932757</v>
+        <v>624689.3595711493</v>
       </c>
       <c r="N2" t="n">
-        <v>801737041.7372</v>
+        <v>10064889.9988</v>
       </c>
       <c r="O2" t="n">
-        <v>784037234.7332001</v>
+        <v>9657149.068700001</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0179990441707403</v>
+        <v>0.01654137501859429</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.018405376413605</v>
+        <v>0.01723977944284353</v>
       </c>
     </row>
     <row r="3">
@@ -578,52 +578,52 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>9666</v>
+        <v>103</v>
       </c>
       <c r="C3" t="n">
-        <v>9648</v>
+        <v>103</v>
       </c>
       <c r="D3" t="n">
-        <v>8554</v>
+        <v>87</v>
       </c>
       <c r="E3" t="n">
-        <v>0.886608623548922</v>
+        <v>0.8446601941747572</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8849575832816057</v>
+        <v>0.8446601941747572</v>
       </c>
       <c r="G3" t="n">
-        <v>0.101949910499804</v>
+        <v>0.1058451956245466</v>
       </c>
       <c r="H3" t="n">
-        <v>0.09022134641168254</v>
+        <v>0.08940322348869467</v>
       </c>
       <c r="I3" t="n">
-        <v>48011620.77939813</v>
+        <v>544119.8952699812</v>
       </c>
       <c r="J3" t="n">
-        <v>17541061.32943826</v>
+        <v>206847.5278420206</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>17541061.32943826</v>
+        <v>206847.5278420206</v>
       </c>
       <c r="M3" t="n">
-        <v>65552682.10883638</v>
+        <v>750967.4231120017</v>
       </c>
       <c r="N3" t="n">
-        <v>837547624.534428</v>
+        <v>10559579.354464</v>
       </c>
       <c r="O3" t="n">
-        <v>820067448.510358</v>
+        <v>10152206.196461</v>
       </c>
       <c r="P3" t="n">
-        <v>0.02094335989453603</v>
+        <v>0.01958861436602368</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.02138977880575723</v>
+        <v>0.02037463816624671</v>
       </c>
     </row>
     <row r="4">
@@ -631,52 +631,52 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>9858</v>
+        <v>104</v>
       </c>
       <c r="C4" t="n">
-        <v>9842</v>
+        <v>104</v>
       </c>
       <c r="D4" t="n">
-        <v>8741</v>
+        <v>86</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8881324933956513</v>
+        <v>0.8269230769230769</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8866910123757354</v>
+        <v>0.8269230769230769</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1061872908635677</v>
+        <v>0.1118823209942627</v>
       </c>
       <c r="H4" t="n">
-        <v>0.09415531643725347</v>
+        <v>0.09251807312987113</v>
       </c>
       <c r="I4" t="n">
-        <v>54607314.52462393</v>
+        <v>618419.5048371302</v>
       </c>
       <c r="J4" t="n">
-        <v>20518986.07138735</v>
+        <v>236910.960031806</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>20518986.07138735</v>
+        <v>236910.960031806</v>
       </c>
       <c r="M4" t="n">
-        <v>75126300.5960113</v>
+        <v>855330.4648689362</v>
       </c>
       <c r="N4" t="n">
-        <v>875630888.769419</v>
+        <v>10924825.81249792</v>
       </c>
       <c r="O4" t="n">
-        <v>858181940.7634652</v>
+        <v>10516481.45975483</v>
       </c>
       <c r="P4" t="n">
-        <v>0.02343337396448407</v>
+        <v>0.02168555948606353</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.02390983204928902</v>
+        <v>0.02252758785706347</v>
       </c>
     </row>
     <row r="5">
@@ -684,52 +684,52 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>10054</v>
+        <v>105</v>
       </c>
       <c r="C5" t="n">
-        <v>10033</v>
+        <v>104</v>
       </c>
       <c r="D5" t="n">
-        <v>8884</v>
+        <v>87</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8854779228545799</v>
+        <v>0.8365384615384616</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8836284066043366</v>
+        <v>0.8285714285714286</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1096290891937461</v>
+        <v>0.1152466813322768</v>
       </c>
       <c r="H5" t="n">
-        <v>0.09687137740175458</v>
+        <v>0.09549010738960079</v>
       </c>
       <c r="I5" t="n">
-        <v>60627454.10565276</v>
+        <v>674928.3527059811</v>
       </c>
       <c r="J5" t="n">
-        <v>23195982.15371279</v>
+        <v>262591.4201946286</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>23195982.15371279</v>
+        <v>262591.4201946286</v>
       </c>
       <c r="M5" t="n">
-        <v>83823436.25936554</v>
+        <v>937519.7729006096</v>
       </c>
       <c r="N5" t="n">
-        <v>914110715.330657</v>
+        <v>11163372.94887286</v>
       </c>
       <c r="O5" t="n">
-        <v>896624609.8676838</v>
+        <v>10752678.26554748</v>
       </c>
       <c r="P5" t="n">
-        <v>0.02537546247373571</v>
+        <v>0.0235225877875147</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.02587033848773776</v>
+        <v>0.02442102457729016</v>
       </c>
     </row>
     <row r="6">
@@ -737,52 +737,52 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>10254</v>
+        <v>106</v>
       </c>
       <c r="C6" t="n">
-        <v>10231</v>
+        <v>106</v>
       </c>
       <c r="D6" t="n">
-        <v>9096</v>
+        <v>89</v>
       </c>
       <c r="E6" t="n">
-        <v>0.889062652722119</v>
+        <v>0.839622641509434</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8870684610883558</v>
+        <v>0.839622641509434</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1086865141011976</v>
+        <v>0.1136698443269339</v>
       </c>
       <c r="H6" t="n">
-        <v>0.09641237880480726</v>
+        <v>0.09543977495374641</v>
       </c>
       <c r="I6" t="n">
-        <v>63928479.04605511</v>
+        <v>706045.9233144443</v>
       </c>
       <c r="J6" t="n">
-        <v>24475449.96408697</v>
+        <v>275089.0228141093</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>24475449.96408697</v>
+        <v>275089.0228141093</v>
       </c>
       <c r="M6" t="n">
-        <v>88403929.01014209</v>
+        <v>981134.9461285535</v>
       </c>
       <c r="N6" t="n">
-        <v>955558181.6979581</v>
+        <v>11682335.88493904</v>
       </c>
       <c r="O6" t="n">
-        <v>937966355.8247766</v>
+        <v>11267870.3611139</v>
       </c>
       <c r="P6" t="n">
-        <v>0.0256137725916342</v>
+        <v>0.02354743310956811</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.02609416618420722</v>
+        <v>0.02441357718877013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add participation flag seeding based on existing deferral rates
</commit_message>
<xml_diff>
--- a/projection_results_AIP_All_Eligible.xlsx
+++ b/projection_results_AIP_All_Eligible.xlsx
@@ -540,37 +540,37 @@
         <v>0.8431372549019608</v>
       </c>
       <c r="G2" t="n">
-        <v>0.09930466255509107</v>
+        <v>0.1064597248414084</v>
       </c>
       <c r="H2" t="n">
-        <v>0.08372746058566501</v>
+        <v>0.08976016016040311</v>
       </c>
       <c r="I2" t="n">
-        <v>458202.2395800996</v>
+        <v>523152.5604975562</v>
       </c>
       <c r="J2" t="n">
-        <v>166487.1199910498</v>
+        <v>198962.2804497781</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>166487.1199910498</v>
+        <v>198962.2804497781</v>
       </c>
       <c r="M2" t="n">
-        <v>624689.3595711493</v>
+        <v>722114.8409473342</v>
       </c>
       <c r="N2" t="n">
-        <v>10064889.9988</v>
+        <v>10195939.0888</v>
       </c>
       <c r="O2" t="n">
-        <v>9657149.068700001</v>
+        <v>9788198.158699997</v>
       </c>
       <c r="P2" t="n">
-        <v>0.01654137501859429</v>
+        <v>0.01951387495717128</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.01723977944284353</v>
+        <v>0.02032675240365208</v>
       </c>
     </row>
     <row r="3">
@@ -584,46 +584,46 @@
         <v>103</v>
       </c>
       <c r="D3" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8446601941747572</v>
+        <v>0.8640776699029126</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8446601941747572</v>
+        <v>0.8640776699029126</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1058451956245466</v>
+        <v>0.1097230768598265</v>
       </c>
       <c r="H3" t="n">
-        <v>0.08940322348869467</v>
+        <v>0.09480926058761706</v>
       </c>
       <c r="I3" t="n">
-        <v>544119.8952699812</v>
+        <v>597470.8937858229</v>
       </c>
       <c r="J3" t="n">
-        <v>206847.5278420206</v>
+        <v>233523.0270999415</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>206847.5278420206</v>
+        <v>233523.0270999415</v>
       </c>
       <c r="M3" t="n">
-        <v>750967.4231120017</v>
+        <v>830993.9208857642</v>
       </c>
       <c r="N3" t="n">
-        <v>10559579.354464</v>
+        <v>10483919.652964</v>
       </c>
       <c r="O3" t="n">
-        <v>10152206.196461</v>
+        <v>10076546.494961</v>
       </c>
       <c r="P3" t="n">
-        <v>0.01958861436602368</v>
+        <v>0.02227440068504532</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.02037463816624671</v>
+        <v>0.02317490692041364</v>
       </c>
     </row>
     <row r="4">
@@ -637,46 +637,46 @@
         <v>104</v>
       </c>
       <c r="D4" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8269230769230769</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8269230769230769</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1118823209942627</v>
+        <v>0.1143843363215895</v>
       </c>
       <c r="H4" t="n">
-        <v>0.09251807312987113</v>
+        <v>0.09678674611826801</v>
       </c>
       <c r="I4" t="n">
-        <v>618419.5048371302</v>
+        <v>662421.2148822283</v>
       </c>
       <c r="J4" t="n">
-        <v>236910.960031806</v>
+        <v>258911.8150543551</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>236910.960031806</v>
+        <v>258911.8150543551</v>
       </c>
       <c r="M4" t="n">
-        <v>855330.4648689362</v>
+        <v>921333.0299365834</v>
       </c>
       <c r="N4" t="n">
-        <v>10924825.81249792</v>
+        <v>10944178.12365292</v>
       </c>
       <c r="O4" t="n">
-        <v>10516481.45975483</v>
+        <v>10535833.77090983</v>
       </c>
       <c r="P4" t="n">
-        <v>0.02168555948606353</v>
+        <v>0.02365749279014258</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.02252758785706347</v>
+        <v>0.02457440205342159</v>
       </c>
     </row>
     <row r="5">
@@ -687,49 +687,49 @@
         <v>105</v>
       </c>
       <c r="C5" t="n">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D5" t="n">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8365384615384616</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8285714285714286</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1152466813322768</v>
+        <v>0.1137241401623681</v>
       </c>
       <c r="H5" t="n">
-        <v>0.09549010738960079</v>
+        <v>0.09747783442488696</v>
       </c>
       <c r="I5" t="n">
-        <v>674928.3527059811</v>
+        <v>688290.7332236361</v>
       </c>
       <c r="J5" t="n">
-        <v>262591.4201946286</v>
+        <v>269272.6104534561</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>262591.4201946286</v>
+        <v>269272.6104534561</v>
       </c>
       <c r="M5" t="n">
-        <v>937519.7729006096</v>
+        <v>957563.3436770922</v>
       </c>
       <c r="N5" t="n">
-        <v>11163372.94887286</v>
+        <v>11180172.36496251</v>
       </c>
       <c r="O5" t="n">
-        <v>10752678.26554748</v>
+        <v>10769477.68163713</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0235225877875147</v>
+        <v>0.0240848353373628</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.02442102457729016</v>
+        <v>0.02500331199094166</v>
       </c>
     </row>
     <row r="6">
@@ -743,46 +743,46 @@
         <v>106</v>
       </c>
       <c r="D6" t="n">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E6" t="n">
-        <v>0.839622641509434</v>
+        <v>0.8679245283018868</v>
       </c>
       <c r="F6" t="n">
-        <v>0.839622641509434</v>
+        <v>0.8679245283018868</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1136698443269339</v>
+        <v>0.111601472672212</v>
       </c>
       <c r="H6" t="n">
-        <v>0.09543977495374641</v>
+        <v>0.09686165552682552</v>
       </c>
       <c r="I6" t="n">
-        <v>706045.9233144443</v>
+        <v>716003.1770682526</v>
       </c>
       <c r="J6" t="n">
-        <v>275089.0228141093</v>
+        <v>280067.6496910135</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>275089.0228141093</v>
+        <v>280067.6496910135</v>
       </c>
       <c r="M6" t="n">
-        <v>981134.9461285535</v>
+        <v>996070.826759266</v>
       </c>
       <c r="N6" t="n">
-        <v>11682335.88493904</v>
+        <v>11684749.18171138</v>
       </c>
       <c r="O6" t="n">
-        <v>11267870.3611139</v>
+        <v>11270283.65788624</v>
       </c>
       <c r="P6" t="n">
-        <v>0.02354743310956811</v>
+        <v>0.02396864882041002</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.02441357718877013</v>
+        <v>0.02485009767212377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove unused imports from utils/__init__.py
</commit_message>
<xml_diff>
--- a/projection_results_AIP_All_Eligible.xlsx
+++ b/projection_results_AIP_All_Eligible.xlsx
@@ -531,46 +531,46 @@
         <v>102</v>
       </c>
       <c r="D2" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8431372549019608</v>
+        <v>0.8529411764705882</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8431372549019608</v>
+        <v>0.8529411764705882</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1064597248414084</v>
+        <v>0.105155020195745</v>
       </c>
       <c r="H2" t="n">
-        <v>0.08976016016040311</v>
+        <v>0.08969104663754716</v>
       </c>
       <c r="I2" t="n">
-        <v>523152.5604975562</v>
+        <v>519414.7856197282</v>
       </c>
       <c r="J2" t="n">
-        <v>198962.2804497781</v>
+        <v>197093.3930108641</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>198962.2804497781</v>
+        <v>197093.3930108641</v>
       </c>
       <c r="M2" t="n">
-        <v>722114.8409473342</v>
+        <v>716508.1786305922</v>
       </c>
       <c r="N2" t="n">
-        <v>10195939.0888</v>
+        <v>10094300.9488</v>
       </c>
       <c r="O2" t="n">
-        <v>9788198.158699997</v>
+        <v>9686560.0187</v>
       </c>
       <c r="P2" t="n">
-        <v>0.01951387495717128</v>
+        <v>0.01952521467415674</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.02032675240365208</v>
+        <v>0.02034709872548907</v>
       </c>
     </row>
     <row r="3">
@@ -581,49 +581,49 @@
         <v>103</v>
       </c>
       <c r="C3" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D3" t="n">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8640776699029126</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8640776699029126</v>
+        <v>0.8252427184466019</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1097230768598265</v>
+        <v>0.1124218121923839</v>
       </c>
       <c r="H3" t="n">
-        <v>0.09480926058761706</v>
+        <v>0.09277528190633627</v>
       </c>
       <c r="I3" t="n">
-        <v>597470.8937858229</v>
+        <v>589272.077115087</v>
       </c>
       <c r="J3" t="n">
-        <v>233523.0270999415</v>
+        <v>229423.6187645734</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>233523.0270999415</v>
+        <v>229423.6187645734</v>
       </c>
       <c r="M3" t="n">
-        <v>830993.9208857642</v>
+        <v>818695.6958796604</v>
       </c>
       <c r="N3" t="n">
-        <v>10483919.652964</v>
+        <v>10505163.513564</v>
       </c>
       <c r="O3" t="n">
-        <v>10076546.494961</v>
+        <v>10097790.355561</v>
       </c>
       <c r="P3" t="n">
-        <v>0.02227440068504532</v>
+        <v>0.02183912877399267</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.02317490692041364</v>
+        <v>0.02272018042424762</v>
       </c>
     </row>
     <row r="4">
@@ -637,46 +637,46 @@
         <v>104</v>
       </c>
       <c r="D4" t="n">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8461538461538461</v>
+        <v>0.8076923076923077</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8461538461538461</v>
+        <v>0.8076923076923077</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1143843363215895</v>
+        <v>0.1180246687376596</v>
       </c>
       <c r="H4" t="n">
-        <v>0.09678674611826801</v>
+        <v>0.09532761705734048</v>
       </c>
       <c r="I4" t="n">
-        <v>662421.2148822283</v>
+        <v>649734.5660466086</v>
       </c>
       <c r="J4" t="n">
-        <v>258911.8150543551</v>
+        <v>252568.4906365452</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>258911.8150543551</v>
+        <v>252568.4906365452</v>
       </c>
       <c r="M4" t="n">
-        <v>921333.0299365834</v>
+        <v>902303.0566831537</v>
       </c>
       <c r="N4" t="n">
-        <v>10944178.12365292</v>
+        <v>10901225.88937092</v>
       </c>
       <c r="O4" t="n">
-        <v>10535833.77090983</v>
+        <v>10492881.53662783</v>
       </c>
       <c r="P4" t="n">
-        <v>0.02365749279014258</v>
+        <v>0.02316881543412548</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.02457440205342159</v>
+        <v>0.02407046050743035</v>
       </c>
     </row>
     <row r="5">
@@ -699,37 +699,37 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1137241401623681</v>
+        <v>0.1126370358327302</v>
       </c>
       <c r="H5" t="n">
-        <v>0.09747783442488696</v>
+        <v>0.09654603071376873</v>
       </c>
       <c r="I5" t="n">
-        <v>688290.7332236361</v>
+        <v>692419.1877078008</v>
       </c>
       <c r="J5" t="n">
-        <v>269272.6104534561</v>
+        <v>271336.8376955385</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>269272.6104534561</v>
+        <v>271336.8376955385</v>
       </c>
       <c r="M5" t="n">
-        <v>957563.3436770922</v>
+        <v>963756.0254033392</v>
       </c>
       <c r="N5" t="n">
-        <v>11180172.36496251</v>
+        <v>11465708.21445205</v>
       </c>
       <c r="O5" t="n">
-        <v>10769477.68163713</v>
+        <v>11055013.53112666</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0240848353373628</v>
+        <v>0.0236650743783563</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.02500331199094166</v>
+        <v>0.02454423388370882</v>
       </c>
     </row>
     <row r="6">
@@ -743,46 +743,46 @@
         <v>106</v>
       </c>
       <c r="D6" t="n">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8679245283018868</v>
+        <v>0.8490566037735849</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8679245283018868</v>
+        <v>0.8490566037735849</v>
       </c>
       <c r="G6" t="n">
-        <v>0.111601472672212</v>
+        <v>0.1130249947913053</v>
       </c>
       <c r="H6" t="n">
-        <v>0.09686165552682552</v>
+        <v>0.09596461821903285</v>
       </c>
       <c r="I6" t="n">
-        <v>716003.1770682526</v>
+        <v>711267.298988305</v>
       </c>
       <c r="J6" t="n">
-        <v>280067.6496910135</v>
+        <v>277699.7106510397</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>280067.6496910135</v>
+        <v>277699.7106510397</v>
       </c>
       <c r="M6" t="n">
-        <v>996070.826759266</v>
+        <v>988967.0096393448</v>
       </c>
       <c r="N6" t="n">
-        <v>11684749.18171138</v>
+        <v>11792951.18548561</v>
       </c>
       <c r="O6" t="n">
-        <v>11270283.65788624</v>
+        <v>11378485.66166047</v>
       </c>
       <c r="P6" t="n">
-        <v>0.02396864882041002</v>
+        <v>0.02354794031478937</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.02485009767212377</v>
+        <v>0.02440568269877443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update auto-increase logic to support new hire only and all eligible scenarios
</commit_message>
<xml_diff>
--- a/projection_results_AIP_All_Eligible.xlsx
+++ b/projection_results_AIP_All_Eligible.xlsx
@@ -540,37 +540,37 @@
         <v>0.8529411764705882</v>
       </c>
       <c r="G2" t="n">
-        <v>0.105155020195745</v>
+        <v>0.1065069431212171</v>
       </c>
       <c r="H2" t="n">
-        <v>0.08969104663754716</v>
+        <v>0.09084415736809691</v>
       </c>
       <c r="I2" t="n">
-        <v>519414.7856197282</v>
+        <v>528276.0912988938</v>
       </c>
       <c r="J2" t="n">
-        <v>197093.3930108641</v>
+        <v>201524.0458504469</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>197093.3930108641</v>
+        <v>201524.0458504469</v>
       </c>
       <c r="M2" t="n">
-        <v>716508.1786305922</v>
+        <v>729800.1371493406</v>
       </c>
       <c r="N2" t="n">
-        <v>10094300.9488</v>
+        <v>10161399.9688</v>
       </c>
       <c r="O2" t="n">
-        <v>9686560.0187</v>
+        <v>9753659.038699998</v>
       </c>
       <c r="P2" t="n">
-        <v>0.01952521467415674</v>
+        <v>0.01983231114504054</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.02034709872548907</v>
+        <v>0.02066137898104204</v>
       </c>
     </row>
     <row r="3">
@@ -581,49 +581,49 @@
         <v>103</v>
       </c>
       <c r="C3" t="n">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D3" t="n">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8543689320388349</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8252427184466019</v>
+        <v>0.8543689320388349</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1124218121923839</v>
+        <v>0.1101170774262103</v>
       </c>
       <c r="H3" t="n">
-        <v>0.09277528190633627</v>
+        <v>0.094080609839869</v>
       </c>
       <c r="I3" t="n">
-        <v>589272.077115087</v>
+        <v>595699.0697549444</v>
       </c>
       <c r="J3" t="n">
-        <v>229423.6187645734</v>
+        <v>232637.1150845023</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>229423.6187645734</v>
+        <v>232637.1150845023</v>
       </c>
       <c r="M3" t="n">
-        <v>818695.6958796604</v>
+        <v>828336.1848394468</v>
       </c>
       <c r="N3" t="n">
-        <v>10505163.513564</v>
+        <v>10536239.823564</v>
       </c>
       <c r="O3" t="n">
-        <v>10097790.355561</v>
+        <v>10128866.665561</v>
       </c>
       <c r="P3" t="n">
-        <v>0.02183912877399267</v>
+        <v>0.02207970955294848</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.02272018042424762</v>
+        <v>0.0229677339791122</v>
       </c>
     </row>
     <row r="4">
@@ -634,49 +634,49 @@
         <v>104</v>
       </c>
       <c r="C4" t="n">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" t="n">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8076923076923077</v>
+        <v>0.8446601941747572</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8076923076923077</v>
+        <v>0.8365384615384616</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1180246687376596</v>
+        <v>0.1155345313075407</v>
       </c>
       <c r="H4" t="n">
-        <v>0.09532761705734048</v>
+        <v>0.09664907907457733</v>
       </c>
       <c r="I4" t="n">
-        <v>649734.5660466086</v>
+        <v>659315.5951792673</v>
       </c>
       <c r="J4" t="n">
-        <v>252568.4906365452</v>
+        <v>257359.0052028746</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>252568.4906365452</v>
+        <v>257359.0052028746</v>
       </c>
       <c r="M4" t="n">
-        <v>902303.0566831537</v>
+        <v>916674.600382142</v>
       </c>
       <c r="N4" t="n">
-        <v>10901225.88937092</v>
+        <v>10860875.61657092</v>
       </c>
       <c r="O4" t="n">
-        <v>10492881.53662783</v>
+        <v>10452531.26382783</v>
       </c>
       <c r="P4" t="n">
-        <v>0.02316881543412548</v>
+        <v>0.02369597206418703</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.02407046050743035</v>
+        <v>0.02462169198129975</v>
       </c>
     </row>
     <row r="5">
@@ -690,46 +690,46 @@
         <v>105</v>
       </c>
       <c r="D5" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.8095238095238095</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.8095238095238095</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1126370358327302</v>
+        <v>0.1172245253426888</v>
       </c>
       <c r="H5" t="n">
-        <v>0.09654603071376873</v>
+        <v>0.09489604432503375</v>
       </c>
       <c r="I5" t="n">
-        <v>692419.1877078008</v>
+        <v>678472.9241290929</v>
       </c>
       <c r="J5" t="n">
-        <v>271336.8376955385</v>
+        <v>264363.7059061846</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>271336.8376955385</v>
+        <v>264363.7059061846</v>
       </c>
       <c r="M5" t="n">
-        <v>963756.0254033392</v>
+        <v>942836.6300352775</v>
       </c>
       <c r="N5" t="n">
-        <v>11465708.21445205</v>
+        <v>11360984.84936805</v>
       </c>
       <c r="O5" t="n">
-        <v>11055013.53112666</v>
+        <v>10950290.16604267</v>
       </c>
       <c r="P5" t="n">
-        <v>0.0236650743783563</v>
+        <v>0.02326943565292139</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.02454423388370882</v>
+        <v>0.02414216444473664</v>
       </c>
     </row>
     <row r="6">
@@ -740,49 +740,49 @@
         <v>106</v>
       </c>
       <c r="C6" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D6" t="n">
         <v>90</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8490566037735849</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="F6" t="n">
         <v>0.8490566037735849</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1130249947913053</v>
+        <v>0.1134076443070747</v>
       </c>
       <c r="H6" t="n">
-        <v>0.09596461821903285</v>
+        <v>0.09628950931732752</v>
       </c>
       <c r="I6" t="n">
-        <v>711267.298988305</v>
+        <v>716159.0169867697</v>
       </c>
       <c r="J6" t="n">
-        <v>277699.7106510397</v>
+        <v>280145.5696502721</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>277699.7106510397</v>
+        <v>280145.5696502721</v>
       </c>
       <c r="M6" t="n">
-        <v>988967.0096393448</v>
+        <v>996304.5866370418</v>
       </c>
       <c r="N6" t="n">
-        <v>11792951.18548561</v>
+        <v>11698901.34244909</v>
       </c>
       <c r="O6" t="n">
-        <v>11378485.66166047</v>
+        <v>11284435.81862395</v>
       </c>
       <c r="P6" t="n">
-        <v>0.02354794031478937</v>
+        <v>0.02394631439738472</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.02440568269877443</v>
+        <v>0.02482583747677638</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add prorated compensation for terminated employees and randomize term dates
</commit_message>
<xml_diff>
--- a/projection_results_AIP_All_Eligible.xlsx
+++ b/projection_results_AIP_All_Eligible.xlsx
@@ -528,49 +528,49 @@
         <v>102</v>
       </c>
       <c r="C2" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D2" t="n">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8529411764705882</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8529411764705882</v>
+        <v>0.9901960784313726</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1065069431212171</v>
+        <v>0.09250231417550324</v>
       </c>
       <c r="H2" t="n">
-        <v>0.09084415736809691</v>
+        <v>0.09159542874241007</v>
       </c>
       <c r="I2" t="n">
-        <v>528276.0912988938</v>
+        <v>538620.5426134155</v>
       </c>
       <c r="J2" t="n">
-        <v>201524.0458504469</v>
+        <v>206696.2715077078</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>201524.0458504469</v>
+        <v>206696.2715077078</v>
       </c>
       <c r="M2" t="n">
-        <v>729800.1371493406</v>
+        <v>745316.8141211235</v>
       </c>
       <c r="N2" t="n">
-        <v>10161399.9688</v>
+        <v>10110406.7188</v>
       </c>
       <c r="O2" t="n">
-        <v>9753659.038699998</v>
+        <v>9702665.788699999</v>
       </c>
       <c r="P2" t="n">
-        <v>0.01983231114504054</v>
+        <v>0.02044391261959444</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.02066137898104204</v>
+        <v>0.02130303939237319</v>
       </c>
     </row>
     <row r="3">
@@ -581,49 +581,49 @@
         <v>103</v>
       </c>
       <c r="C3" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D3" t="n">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8543689320388349</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8543689320388349</v>
+        <v>0.9902912621359223</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1101170774262103</v>
+        <v>0.09875808338513453</v>
       </c>
       <c r="H3" t="n">
-        <v>0.094080609839869</v>
+        <v>0.09779926704158953</v>
       </c>
       <c r="I3" t="n">
-        <v>595699.0697549444</v>
+        <v>638784.0023400235</v>
       </c>
       <c r="J3" t="n">
-        <v>232637.1150845023</v>
+        <v>254179.5813770418</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>232637.1150845023</v>
+        <v>254179.5813770418</v>
       </c>
       <c r="M3" t="n">
-        <v>828336.1848394468</v>
+        <v>892963.5837170655</v>
       </c>
       <c r="N3" t="n">
-        <v>10536239.823564</v>
+        <v>10480889.176664</v>
       </c>
       <c r="O3" t="n">
-        <v>10128866.665561</v>
+        <v>10073516.018661</v>
       </c>
       <c r="P3" t="n">
-        <v>0.02207970955294848</v>
+        <v>0.02425171920937585</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.0229677339791122</v>
+        <v>0.02523245914397504</v>
       </c>
     </row>
     <row r="4">
@@ -634,49 +634,49 @@
         <v>104</v>
       </c>
       <c r="C4" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D4" t="n">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8446601941747572</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8365384615384616</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1155345313075407</v>
+        <v>0.1018639034285131</v>
       </c>
       <c r="H4" t="n">
-        <v>0.09664907907457733</v>
+        <v>0.1018639034285131</v>
       </c>
       <c r="I4" t="n">
-        <v>659315.5951792673</v>
+        <v>719445.6476580924</v>
       </c>
       <c r="J4" t="n">
-        <v>257359.0052028746</v>
+        <v>287424.0314422871</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>257359.0052028746</v>
+        <v>287424.0314422871</v>
       </c>
       <c r="M4" t="n">
-        <v>916674.600382142</v>
+        <v>1006869.67910038</v>
       </c>
       <c r="N4" t="n">
-        <v>10860875.61657092</v>
+        <v>10862870.64886392</v>
       </c>
       <c r="O4" t="n">
-        <v>10452531.26382783</v>
+        <v>10454526.29612083</v>
       </c>
       <c r="P4" t="n">
-        <v>0.02369597206418703</v>
+        <v>0.0264593071880449</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.02462169198129975</v>
+        <v>0.02749278382406827</v>
       </c>
     </row>
     <row r="5">
@@ -690,46 +690,46 @@
         <v>105</v>
       </c>
       <c r="D5" t="n">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8095238095238095</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8095238095238095</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1172245253426888</v>
+        <v>0.1034799091691537</v>
       </c>
       <c r="H5" t="n">
-        <v>0.09489604432503375</v>
+        <v>0.1034799091691537</v>
       </c>
       <c r="I5" t="n">
-        <v>678472.9241290929</v>
+        <v>770434.6693487333</v>
       </c>
       <c r="J5" t="n">
-        <v>264363.7059061846</v>
+        <v>310344.5785160048</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>264363.7059061846</v>
+        <v>310344.5785160048</v>
       </c>
       <c r="M5" t="n">
-        <v>942836.6300352775</v>
+        <v>1080779.247864738</v>
       </c>
       <c r="N5" t="n">
-        <v>11360984.84936805</v>
+        <v>11340380.44192984</v>
       </c>
       <c r="O5" t="n">
-        <v>10950290.16604267</v>
+        <v>10929685.75860446</v>
       </c>
       <c r="P5" t="n">
-        <v>0.02326943565292139</v>
+        <v>0.02736632867875746</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.02414216444473664</v>
+        <v>0.02839464787646656</v>
       </c>
     </row>
     <row r="6">
@@ -740,49 +740,49 @@
         <v>106</v>
       </c>
       <c r="C6" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D6" t="n">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8571428571428571</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8490566037735849</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1134076443070747</v>
+        <v>0.1038456560215263</v>
       </c>
       <c r="H6" t="n">
-        <v>0.09628950931732752</v>
+        <v>0.1038456560215263</v>
       </c>
       <c r="I6" t="n">
-        <v>716159.0169867697</v>
+        <v>810410.2254774929</v>
       </c>
       <c r="J6" t="n">
-        <v>280145.5696502721</v>
+        <v>327271.1738956337</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>280145.5696502721</v>
+        <v>327271.1738956337</v>
       </c>
       <c r="M6" t="n">
-        <v>996304.5866370418</v>
+        <v>1137681.399373127</v>
       </c>
       <c r="N6" t="n">
-        <v>11698901.34244909</v>
+        <v>11677572.73988773</v>
       </c>
       <c r="O6" t="n">
-        <v>11284435.81862395</v>
+        <v>11263107.21606259</v>
       </c>
       <c r="P6" t="n">
-        <v>0.02394631439738472</v>
+        <v>0.02802561638325363</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.02482583747677638</v>
+        <v>0.0290569172092142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update projection outputs and fix termination compensation proration logic
</commit_message>
<xml_diff>
--- a/projection_results_AIP_All_Eligible.xlsx
+++ b/projection_results_AIP_All_Eligible.xlsx
@@ -528,49 +528,49 @@
         <v>102</v>
       </c>
       <c r="C2" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D2" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9901960784313726</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0.09250231417550324</v>
+        <v>0.09127332586241999</v>
       </c>
       <c r="H2" t="n">
-        <v>0.09159542874241007</v>
+        <v>0.09127332586241999</v>
       </c>
       <c r="I2" t="n">
-        <v>538620.5426134155</v>
+        <v>544219.5395527922</v>
       </c>
       <c r="J2" t="n">
-        <v>206696.2715077078</v>
+        <v>209495.769977396</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>206696.2715077078</v>
+        <v>209495.769977396</v>
       </c>
       <c r="M2" t="n">
-        <v>745316.8141211235</v>
+        <v>753715.3095301883</v>
       </c>
       <c r="N2" t="n">
-        <v>10110406.7188</v>
+        <v>10316742.6388</v>
       </c>
       <c r="O2" t="n">
-        <v>9702665.788699999</v>
+        <v>9909001.708699998</v>
       </c>
       <c r="P2" t="n">
-        <v>0.02044391261959444</v>
+        <v>0.02030638713323217</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.02130303939237319</v>
+        <v>0.02114196526916137</v>
       </c>
     </row>
     <row r="3">
@@ -578,52 +578,52 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C3" t="n">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D3" t="n">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9902912621359223</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>0.09875808338513453</v>
+        <v>0.09717788792471758</v>
       </c>
       <c r="H3" t="n">
-        <v>0.09779926704158953</v>
+        <v>0.09717788792471758</v>
       </c>
       <c r="I3" t="n">
-        <v>638784.0023400235</v>
+        <v>654630.7013274725</v>
       </c>
       <c r="J3" t="n">
-        <v>254179.5813770418</v>
+        <v>262102.9308707663</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>254179.5813770418</v>
+        <v>262102.9308707663</v>
       </c>
       <c r="M3" t="n">
-        <v>892963.5837170655</v>
+        <v>916733.6321982386</v>
       </c>
       <c r="N3" t="n">
-        <v>10480889.176664</v>
+        <v>10760730.661864</v>
       </c>
       <c r="O3" t="n">
-        <v>10073516.018661</v>
+        <v>10353357.503861</v>
       </c>
       <c r="P3" t="n">
-        <v>0.02425171920937585</v>
+        <v>0.02435735444988493</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.02523245914397504</v>
+        <v>0.02531574233508523</v>
       </c>
     </row>
     <row r="4">
@@ -631,13 +631,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C4" t="n">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D4" t="n">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
@@ -646,37 +646,37 @@
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1018639034285131</v>
+        <v>0.09963069641345117</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1018639034285131</v>
+        <v>0.09963069641345117</v>
       </c>
       <c r="I4" t="n">
-        <v>719445.6476580924</v>
+        <v>734817.7333005213</v>
       </c>
       <c r="J4" t="n">
-        <v>287424.0314422871</v>
+        <v>295110.0742635016</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>287424.0314422871</v>
+        <v>295110.0742635016</v>
       </c>
       <c r="M4" t="n">
-        <v>1006869.67910038</v>
+        <v>1029927.807564023</v>
       </c>
       <c r="N4" t="n">
-        <v>10862870.64886392</v>
+        <v>11223740.87971992</v>
       </c>
       <c r="O4" t="n">
-        <v>10454526.29612083</v>
+        <v>10815396.52697683</v>
       </c>
       <c r="P4" t="n">
-        <v>0.0264593071880449</v>
+        <v>0.02629337913500242</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.02749278382406827</v>
+        <v>0.02728610768245148</v>
       </c>
     </row>
     <row r="5">
@@ -684,13 +684,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C5" t="n">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D5" t="n">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -699,37 +699,37 @@
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1034799091691537</v>
+        <v>0.1015414746775767</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1034799091691537</v>
+        <v>0.1015414746775767</v>
       </c>
       <c r="I5" t="n">
-        <v>770434.6693487333</v>
+        <v>781388.0653614923</v>
       </c>
       <c r="J5" t="n">
-        <v>310344.5785160048</v>
+        <v>315821.2765223843</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>310344.5785160048</v>
+        <v>315821.2765223843</v>
       </c>
       <c r="M5" t="n">
-        <v>1080779.247864738</v>
+        <v>1097209.341883876</v>
       </c>
       <c r="N5" t="n">
-        <v>11340380.44192984</v>
+        <v>11501137.06941152</v>
       </c>
       <c r="O5" t="n">
-        <v>10929685.75860446</v>
+        <v>11090442.38608613</v>
       </c>
       <c r="P5" t="n">
-        <v>0.02736632867875746</v>
+        <v>0.02746000457314296</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.02839464787646656</v>
+        <v>0.02847688717256292</v>
       </c>
     </row>
     <row r="6">
@@ -737,13 +737,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C6" t="n">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D6" t="n">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
@@ -752,37 +752,37 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1038456560215263</v>
+        <v>0.1022024053100728</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1038456560215263</v>
+        <v>0.1022024053100728</v>
       </c>
       <c r="I6" t="n">
-        <v>810410.2254774929</v>
+        <v>827577.8738163244</v>
       </c>
       <c r="J6" t="n">
-        <v>327271.1738956337</v>
+        <v>335854.9980650494</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>327271.1738956337</v>
+        <v>335854.9980650494</v>
       </c>
       <c r="M6" t="n">
-        <v>1137681.399373127</v>
+        <v>1163432.871881374</v>
       </c>
       <c r="N6" t="n">
-        <v>11677572.73988773</v>
+        <v>11926849.94239386</v>
       </c>
       <c r="O6" t="n">
-        <v>11263107.21606259</v>
+        <v>11512384.41856872</v>
       </c>
       <c r="P6" t="n">
-        <v>0.02802561638325363</v>
+        <v>0.02815957270253366</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.0290569172092142</v>
+        <v>0.02917336546921916</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update projection files with new auto-enrollment and auto-increase results
</commit_message>
<xml_diff>
--- a/projection_results_AIP_All_Eligible.xlsx
+++ b/projection_results_AIP_All_Eligible.xlsx
@@ -525,52 +525,52 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>102</v>
+        <v>9478</v>
       </c>
       <c r="C2" t="n">
-        <v>102</v>
+        <v>9456</v>
       </c>
       <c r="D2" t="n">
-        <v>102</v>
+        <v>9456</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0.9976788351972991</v>
       </c>
       <c r="G2" t="n">
-        <v>0.09127332586241999</v>
+        <v>0.09258994317483452</v>
       </c>
       <c r="H2" t="n">
-        <v>0.09127332586241999</v>
+        <v>0.092375026657653</v>
       </c>
       <c r="I2" t="n">
-        <v>544219.5395527922</v>
+        <v>47112440.0389384</v>
       </c>
       <c r="J2" t="n">
-        <v>209495.769977396</v>
+        <v>17356555.7788052</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>209495.769977396</v>
+        <v>17356555.7788052</v>
       </c>
       <c r="M2" t="n">
-        <v>753715.3095301883</v>
+        <v>64468995.81774361</v>
       </c>
       <c r="N2" t="n">
-        <v>10316742.6388</v>
+        <v>813109489.4172001</v>
       </c>
       <c r="O2" t="n">
-        <v>9909001.708699998</v>
+        <v>794833158.7732</v>
       </c>
       <c r="P2" t="n">
-        <v>0.02030638713323217</v>
+        <v>0.02134590237194943</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.02114196526916137</v>
+        <v>0.02183672835893573</v>
       </c>
     </row>
     <row r="3">
@@ -578,52 +578,52 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>106</v>
+        <v>9762</v>
       </c>
       <c r="C3" t="n">
-        <v>106</v>
+        <v>9738</v>
       </c>
       <c r="D3" t="n">
-        <v>106</v>
+        <v>9738</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0.9975414874001229</v>
       </c>
       <c r="G3" t="n">
-        <v>0.09717788792471758</v>
+        <v>0.09761071208907925</v>
       </c>
       <c r="H3" t="n">
-        <v>0.09717788792471758</v>
+        <v>0.09737073492352527</v>
       </c>
       <c r="I3" t="n">
-        <v>654630.7013274725</v>
+        <v>55505811.34755692</v>
       </c>
       <c r="J3" t="n">
-        <v>262102.9308707663</v>
+        <v>21282186.73698258</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>262102.9308707663</v>
+        <v>21282186.73698258</v>
       </c>
       <c r="M3" t="n">
-        <v>916733.6321982386</v>
+        <v>76787998.0845395</v>
       </c>
       <c r="N3" t="n">
-        <v>10760730.661864</v>
+        <v>863794315.9995871</v>
       </c>
       <c r="O3" t="n">
-        <v>10353357.503861</v>
+        <v>845379885.828617</v>
       </c>
       <c r="P3" t="n">
-        <v>0.02435735444988493</v>
+        <v>0.0246380259082334</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.02531574233508523</v>
+        <v>0.0251747020407546</v>
       </c>
     </row>
     <row r="4">
@@ -631,52 +631,52 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>108</v>
+        <v>10046</v>
       </c>
       <c r="C4" t="n">
-        <v>108</v>
+        <v>10024</v>
       </c>
       <c r="D4" t="n">
-        <v>108</v>
+        <v>10024</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0.9978100736611587</v>
       </c>
       <c r="G4" t="n">
-        <v>0.09963069641345117</v>
+        <v>0.1008389917673471</v>
       </c>
       <c r="H4" t="n">
-        <v>0.09963069641345117</v>
+        <v>0.1006181618032936</v>
       </c>
       <c r="I4" t="n">
-        <v>734817.7333005213</v>
+        <v>62994171.20052955</v>
       </c>
       <c r="J4" t="n">
-        <v>295110.0742635016</v>
+        <v>24707287.94181236</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>295110.0742635016</v>
+        <v>24707287.94181236</v>
       </c>
       <c r="M4" t="n">
-        <v>1029927.807564023</v>
+        <v>87701459.1423419</v>
       </c>
       <c r="N4" t="n">
-        <v>11223740.87971992</v>
+        <v>916693029.3738154</v>
       </c>
       <c r="O4" t="n">
-        <v>10815396.52697683</v>
+        <v>897970254.2003546</v>
       </c>
       <c r="P4" t="n">
-        <v>0.02629337913500242</v>
+        <v>0.02695262988820771</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.02728610768245148</v>
+        <v>0.02751459508401454</v>
       </c>
     </row>
     <row r="5">
@@ -684,52 +684,52 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>109</v>
+        <v>10337</v>
       </c>
       <c r="C5" t="n">
-        <v>109</v>
+        <v>10309</v>
       </c>
       <c r="D5" t="n">
-        <v>109</v>
+        <v>10309</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0.9972912837380284</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1015414746775767</v>
+        <v>0.1007746111987947</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1015414746775767</v>
+        <v>0.1005016413706467</v>
       </c>
       <c r="I5" t="n">
-        <v>781388.0653614923</v>
+        <v>67918402.13472392</v>
       </c>
       <c r="J5" t="n">
-        <v>315821.2765223843</v>
+        <v>26836175.90669475</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>315821.2765223843</v>
+        <v>26836175.90669475</v>
       </c>
       <c r="M5" t="n">
-        <v>1097209.341883876</v>
+        <v>94754578.04141869</v>
       </c>
       <c r="N5" t="n">
-        <v>11501137.06941152</v>
+        <v>969816544.9170408</v>
       </c>
       <c r="O5" t="n">
-        <v>11090442.38608613</v>
+        <v>951407665.5136355</v>
       </c>
       <c r="P5" t="n">
-        <v>0.02746000457314296</v>
+        <v>0.02767139419032117</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.02847688717256292</v>
+        <v>0.02820681068635992</v>
       </c>
     </row>
     <row r="6">
@@ -737,52 +737,52 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>110</v>
+        <v>10656</v>
       </c>
       <c r="C6" t="n">
-        <v>110</v>
+        <v>10631</v>
       </c>
       <c r="D6" t="n">
-        <v>110</v>
+        <v>10631</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>0.9976539039039038</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1022024053100728</v>
+        <v>0.1002504979019584</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1022024053100728</v>
+        <v>0.1000153006001989</v>
       </c>
       <c r="I6" t="n">
-        <v>827577.8738163244</v>
+        <v>73124236.81502223</v>
       </c>
       <c r="J6" t="n">
-        <v>335854.9980650494</v>
+        <v>29067604.94581254</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>335854.9980650494</v>
+        <v>29067604.94581254</v>
       </c>
       <c r="M6" t="n">
-        <v>1163432.871881374</v>
+        <v>102191841.7608348</v>
       </c>
       <c r="N6" t="n">
-        <v>11926849.94239386</v>
+        <v>1033114253.054143</v>
       </c>
       <c r="O6" t="n">
-        <v>11512384.41856872</v>
+        <v>1014594770.022316</v>
       </c>
       <c r="P6" t="n">
-        <v>0.02815957270253366</v>
+        <v>0.02813590545274296</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.02917336546921916</v>
+        <v>0.02864947248365294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>